<commit_message>
changes in excel src_files
</commit_message>
<xml_diff>
--- a/files/BoucheoCajaBanco.xlsx
+++ b/files/BoucheoCajaBanco.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VS943JJ\Desktop\T440-Eddy\documents\tensorflowjs\sentencesSimilarV2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VS943JJ\Desktop\T440-Eddy\documents\tensorflowjs\sentencesSimilarV2\sentences-tfjs\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7D5C48-8DC7-462E-8E3C-81FF592E5347}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5338F3B3-5BF4-473C-A87F-79C40349C5CD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{5A49478C-0C4E-4A37-99C8-C3CA170CE4B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Caja" sheetId="1" r:id="rId1"/>
-    <sheet name="Banco" sheetId="2" r:id="rId2"/>
+    <sheet name="Bancos" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -271,11 +271,11 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,10 +608,10 @@
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="D1" s="4"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -632,19 +632,19 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>43436</v>
       </c>
       <c r="C3">
         <f ca="1">+RANDBETWEEN(80,12000)</f>
-        <v>11876</v>
+        <v>5078</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>43437</v>
       </c>
       <c r="C4">
@@ -655,7 +655,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>43438</v>
       </c>
       <c r="B5">
@@ -666,7 +666,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>43439</v>
       </c>
       <c r="B6">
@@ -677,7 +677,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>43440</v>
       </c>
       <c r="B7">
@@ -688,7 +688,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>43441</v>
       </c>
       <c r="B8">
@@ -699,7 +699,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>43442</v>
       </c>
       <c r="B9">
@@ -710,67 +710,67 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>43443</v>
       </c>
       <c r="B10">
         <f ca="1">+RANDBETWEEN(90,120)</f>
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>43444</v>
       </c>
       <c r="B11">
-        <f t="shared" ref="B11:B15" ca="1" si="0">+RANDBETWEEN(90,120)</f>
-        <v>101</v>
+        <f t="shared" ref="B11:B14" ca="1" si="0">+RANDBETWEEN(90,120)</f>
+        <v>100</v>
       </c>
       <c r="D11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>43445</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="D12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <v>43446</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="D13" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="3">
+      <c r="A14" s="2">
         <v>43447</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D14" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="3">
+      <c r="A15" s="2">
         <v>43448</v>
       </c>
       <c r="C15">
@@ -781,7 +781,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="3">
+      <c r="A16" s="2">
         <v>43449</v>
       </c>
       <c r="B16">
@@ -792,7 +792,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="3">
+      <c r="A17" s="2">
         <v>43450</v>
       </c>
       <c r="B17">
@@ -803,7 +803,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="3">
+      <c r="A18" s="2">
         <v>43451</v>
       </c>
       <c r="B18">
@@ -814,7 +814,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="3">
+      <c r="A19" s="2">
         <v>43452</v>
       </c>
       <c r="B19">
@@ -825,7 +825,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="3">
+      <c r="A20" s="2">
         <v>43453</v>
       </c>
       <c r="B20">
@@ -836,7 +836,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="3">
+      <c r="A21" s="2">
         <v>43453</v>
       </c>
       <c r="B21">
@@ -847,7 +847,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="3">
+      <c r="A22" s="2">
         <v>43453</v>
       </c>
       <c r="B22">
@@ -884,11 +884,11 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -909,12 +909,12 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>43446</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <f ca="1">+Caja!$C$3/8</f>
-        <v>1484.5</v>
+        <v>634.75</v>
       </c>
       <c r="D3" t="s">
         <v>24</v>
@@ -924,12 +924,12 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>44184</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <f ca="1">+Caja!$C$3/8</f>
-        <v>1484.5</v>
+        <v>634.75</v>
       </c>
       <c r="D4" t="s">
         <v>24</v>
@@ -939,12 +939,12 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>44185</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <f ca="1">+Caja!$C$3/8</f>
-        <v>1484.5</v>
+        <v>634.75</v>
       </c>
       <c r="D5" t="s">
         <v>24</v>
@@ -954,12 +954,12 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>44186</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <f ca="1">+Caja!$C$3/8</f>
-        <v>1484.5</v>
+        <v>634.75</v>
       </c>
       <c r="D6" t="s">
         <v>24</v>
@@ -969,12 +969,12 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>44187</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <f ca="1">+Caja!$C$3/8</f>
-        <v>1484.5</v>
+        <v>634.75</v>
       </c>
       <c r="D7" t="s">
         <v>25</v>
@@ -984,12 +984,12 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>44188</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <f ca="1">+Caja!$C$3/8</f>
-        <v>1484.5</v>
+        <v>634.75</v>
       </c>
       <c r="D8" t="s">
         <v>27</v>
@@ -999,12 +999,12 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>44189</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <f ca="1">+Caja!$C$3/8</f>
-        <v>1484.5</v>
+        <v>634.75</v>
       </c>
       <c r="D9" t="s">
         <v>26</v>
@@ -1014,12 +1014,12 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>44190</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <f ca="1">+Caja!$C$3/8</f>
-        <v>1484.5</v>
+        <v>634.75</v>
       </c>
       <c r="D10" t="s">
         <v>24</v>
@@ -1029,7 +1029,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>44191</v>
       </c>
       <c r="B11">
@@ -1044,7 +1044,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>44192</v>
       </c>
       <c r="B12">
@@ -1058,7 +1058,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <v>44193</v>
       </c>
       <c r="B13">
@@ -1072,7 +1072,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="3">
+      <c r="A14" s="2">
         <v>44194</v>
       </c>
       <c r="B14">
@@ -1086,7 +1086,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="3">
+      <c r="A15" s="2">
         <v>44195</v>
       </c>
       <c r="B15">
@@ -1100,7 +1100,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="3">
+      <c r="A16" s="2">
         <v>44196</v>
       </c>
       <c r="B16">
@@ -1115,12 +1115,12 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="3">
+      <c r="A17" s="2">
         <v>44184</v>
       </c>
       <c r="B17">
         <f ca="1">+Caja!B10</f>
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D17" t="s">
         <v>13</v>
@@ -1130,12 +1130,12 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="3">
+      <c r="A18" s="2">
         <v>44185</v>
       </c>
       <c r="B18">
         <f ca="1">+Caja!$B$11/2</f>
-        <v>50.5</v>
+        <v>50</v>
       </c>
       <c r="D18" t="s">
         <v>14</v>
@@ -1145,12 +1145,12 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="3">
+      <c r="A19" s="2">
         <v>44186</v>
       </c>
       <c r="B19">
         <f ca="1">+Caja!$B$11/2</f>
-        <v>50.5</v>
+        <v>50</v>
       </c>
       <c r="D19" t="s">
         <v>14</v>
@@ -1160,12 +1160,12 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="3">
+      <c r="A20" s="2">
         <v>44187</v>
       </c>
       <c r="B20">
         <f ca="1">+Caja!$B$12/2</f>
-        <v>45.5</v>
+        <v>56.5</v>
       </c>
       <c r="D20" t="s">
         <v>14</v>
@@ -1175,12 +1175,12 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="3">
+      <c r="A21" s="2">
         <v>44188</v>
       </c>
       <c r="B21">
         <f ca="1">+Caja!$B$12/2</f>
-        <v>45.5</v>
+        <v>56.5</v>
       </c>
       <c r="D21" t="s">
         <v>14</v>
@@ -1190,12 +1190,12 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="3">
+      <c r="A22" s="2">
         <v>44189</v>
       </c>
       <c r="B22">
         <f ca="1">+Caja!B13-37</f>
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D22" t="s">
         <v>16</v>
@@ -1205,7 +1205,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="3">
+      <c r="A23" s="2">
         <v>44190</v>
       </c>
       <c r="B23">
@@ -1219,12 +1219,12 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="3">
+      <c r="A24" s="2">
         <v>44191</v>
       </c>
       <c r="B24">
         <f ca="1">+Caja!B14-56</f>
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D24" t="s">
         <v>17</v>
@@ -1234,7 +1234,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="3">
+      <c r="A25" s="2">
         <v>44192</v>
       </c>
       <c r="B25">
@@ -1248,7 +1248,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="3">
+      <c r="A26" s="2">
         <v>44193</v>
       </c>
       <c r="C26">
@@ -1262,7 +1262,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="3">
+      <c r="A27" s="2">
         <v>44194</v>
       </c>
       <c r="B27">
@@ -1276,7 +1276,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="3">
+      <c r="A28" s="2">
         <v>44195</v>
       </c>
       <c r="B28">
@@ -1290,7 +1290,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="3">
+      <c r="A29" s="2">
         <v>44196</v>
       </c>
       <c r="B29">
@@ -1304,7 +1304,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="3">
+      <c r="A30" s="2">
         <v>44184</v>
       </c>
       <c r="B30">
@@ -1318,7 +1318,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="3">
+      <c r="A31" s="2">
         <v>44185</v>
       </c>
       <c r="B31">
@@ -1332,7 +1332,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="3">
+      <c r="A32" s="2">
         <v>44186</v>
       </c>
       <c r="B32">
@@ -1346,7 +1346,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="3">
+      <c r="A33" s="2">
         <v>44187</v>
       </c>
       <c r="B33">
@@ -1360,7 +1360,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="3">
+      <c r="A34" s="2">
         <v>44188</v>
       </c>
       <c r="B34">
@@ -1374,7 +1374,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="3">
+      <c r="A35" s="2">
         <v>44189</v>
       </c>
       <c r="B35">
@@ -1388,7 +1388,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="3">
+      <c r="A36" s="2">
         <v>44190</v>
       </c>
       <c r="B36">
@@ -1402,7 +1402,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="3">
+      <c r="A37" s="2">
         <v>44191</v>
       </c>
       <c r="B37">
@@ -1416,7 +1416,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="3">
+      <c r="A38" s="2">
         <v>44192</v>
       </c>
       <c r="B38">
@@ -1430,7 +1430,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="3">
+      <c r="A39" s="2">
         <v>44193</v>
       </c>
       <c r="B39">
@@ -1444,7 +1444,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="3">
+      <c r="A40" s="2">
         <v>44194</v>
       </c>
       <c r="B40">
@@ -1458,7 +1458,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="3">
+      <c r="A41" s="2">
         <v>44195</v>
       </c>
       <c r="C41">
@@ -1472,7 +1472,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="3">
+      <c r="A42" s="2">
         <v>44196</v>
       </c>
       <c r="B42">
@@ -1486,7 +1486,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="3">
+      <c r="A43" s="2">
         <v>44196</v>
       </c>
       <c r="B43">
@@ -1500,7 +1500,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" s="3">
+      <c r="A44" s="2">
         <v>44196</v>
       </c>
       <c r="B44">

</xml_diff>

<commit_message>
last changes for today
</commit_message>
<xml_diff>
--- a/files/BoucheoCajaBanco.xlsx
+++ b/files/BoucheoCajaBanco.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VS943JJ\Desktop\T440-Eddy\documents\tensorflowjs\sentencesSimilarV2\sentences-tfjs\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VS943JJ\Desktop\T440-Eddy\documents\tensorflowjs\sentencesSimilarV2\sentences-tfjs\src\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5338F3B3-5BF4-473C-A87F-79C40349C5CD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3638615-0F4B-43AE-88BD-D9A58DB0BB36}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{5A49478C-0C4E-4A37-99C8-C3CA170CE4B6}"/>
   </bookViews>
@@ -16,6 +16,9 @@
     <sheet name="Caja" sheetId="1" r:id="rId1"/>
     <sheet name="Bancos" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -291,6 +294,62 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Caja"/>
+      <sheetName val="Bancos"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="C3">
+            <v>1192</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="C4">
+            <v>0.05</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9">
+            <v>75</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10">
+            <v>93</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="B11">
+            <v>106</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="B12">
+            <v>115</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="B13">
+            <v>109</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="B14">
+            <v>114</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -637,7 +696,7 @@
       </c>
       <c r="C3">
         <f ca="1">+RANDBETWEEN(80,12000)</f>
-        <v>5078</v>
+        <v>8317</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -715,7 +774,7 @@
       </c>
       <c r="B10">
         <f ca="1">+RANDBETWEEN(90,120)</f>
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
@@ -727,7 +786,7 @@
       </c>
       <c r="B11">
         <f t="shared" ref="B11:B14" ca="1" si="0">+RANDBETWEEN(90,120)</f>
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D11" t="s">
         <v>14</v>
@@ -739,7 +798,7 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="D12" t="s">
         <v>15</v>
@@ -751,7 +810,7 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D13" t="s">
         <v>16</v>
@@ -763,7 +822,7 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>91</v>
+        <v>119</v>
       </c>
       <c r="D14" t="s">
         <v>17</v>
@@ -871,7 +930,7 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+      <selection activeCell="A2" sqref="A2:E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -913,8 +972,8 @@
         <v>43446</v>
       </c>
       <c r="B3" s="3">
-        <f ca="1">+Caja!$C$3/8</f>
-        <v>634.75</v>
+        <f ca="1">+[1]Caja!$C$3/8</f>
+        <v>149</v>
       </c>
       <c r="D3" t="s">
         <v>24</v>
@@ -928,8 +987,8 @@
         <v>44184</v>
       </c>
       <c r="B4" s="3">
-        <f ca="1">+Caja!$C$3/8</f>
-        <v>634.75</v>
+        <f ca="1">+[1]Caja!$C$3/8</f>
+        <v>149</v>
       </c>
       <c r="D4" t="s">
         <v>24</v>
@@ -943,8 +1002,8 @@
         <v>44185</v>
       </c>
       <c r="B5" s="3">
-        <f ca="1">+Caja!$C$3/8</f>
-        <v>634.75</v>
+        <f ca="1">+[1]Caja!$C$3/8</f>
+        <v>149</v>
       </c>
       <c r="D5" t="s">
         <v>24</v>
@@ -958,8 +1017,8 @@
         <v>44186</v>
       </c>
       <c r="B6" s="3">
-        <f ca="1">+Caja!$C$3/8</f>
-        <v>634.75</v>
+        <f ca="1">+[1]Caja!$C$3/8</f>
+        <v>149</v>
       </c>
       <c r="D6" t="s">
         <v>24</v>
@@ -973,8 +1032,8 @@
         <v>44187</v>
       </c>
       <c r="B7" s="3">
-        <f ca="1">+Caja!$C$3/8</f>
-        <v>634.75</v>
+        <f ca="1">+[1]Caja!$C$3/8</f>
+        <v>149</v>
       </c>
       <c r="D7" t="s">
         <v>25</v>
@@ -988,8 +1047,8 @@
         <v>44188</v>
       </c>
       <c r="B8" s="3">
-        <f ca="1">+Caja!$C$3/8</f>
-        <v>634.75</v>
+        <f ca="1">+[1]Caja!$C$3/8</f>
+        <v>149</v>
       </c>
       <c r="D8" t="s">
         <v>27</v>
@@ -1003,8 +1062,8 @@
         <v>44189</v>
       </c>
       <c r="B9" s="3">
-        <f ca="1">+Caja!$C$3/8</f>
-        <v>634.75</v>
+        <f ca="1">+[1]Caja!$C$3/8</f>
+        <v>149</v>
       </c>
       <c r="D9" t="s">
         <v>26</v>
@@ -1018,8 +1077,8 @@
         <v>44190</v>
       </c>
       <c r="B10" s="3">
-        <f ca="1">+Caja!$C$3/8</f>
-        <v>634.75</v>
+        <f ca="1">+[1]Caja!$C$3/8</f>
+        <v>149</v>
       </c>
       <c r="D10" t="s">
         <v>24</v>
@@ -1033,7 +1092,7 @@
         <v>44191</v>
       </c>
       <c r="B11">
-        <f>+Caja!C4</f>
+        <f>+[1]Caja!C4</f>
         <v>0.05</v>
       </c>
       <c r="D11" t="s">
@@ -1047,7 +1106,7 @@
       <c r="A12" s="2">
         <v>44192</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>90</v>
       </c>
       <c r="D12" t="s">
@@ -1061,7 +1120,7 @@
       <c r="A13" s="2">
         <v>44193</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>65</v>
       </c>
       <c r="D13" t="s">
@@ -1075,7 +1134,7 @@
       <c r="A14" s="2">
         <v>44194</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <v>175</v>
       </c>
       <c r="D14" t="s">
@@ -1089,7 +1148,7 @@
       <c r="A15" s="2">
         <v>44195</v>
       </c>
-      <c r="B15">
+      <c r="C15">
         <v>89</v>
       </c>
       <c r="D15" t="s">
@@ -1103,8 +1162,8 @@
       <c r="A16" s="2">
         <v>44196</v>
       </c>
-      <c r="B16">
-        <f>+Caja!B9</f>
+      <c r="C16">
+        <f>+[1]Caja!B9</f>
         <v>75</v>
       </c>
       <c r="D16" t="s">
@@ -1118,9 +1177,9 @@
       <c r="A17" s="2">
         <v>44184</v>
       </c>
-      <c r="B17">
-        <f ca="1">+Caja!B10</f>
-        <v>105</v>
+      <c r="C17">
+        <f ca="1">+[1]Caja!B10</f>
+        <v>93</v>
       </c>
       <c r="D17" t="s">
         <v>13</v>
@@ -1133,9 +1192,9 @@
       <c r="A18" s="2">
         <v>44185</v>
       </c>
-      <c r="B18">
-        <f ca="1">+Caja!$B$11/2</f>
-        <v>50</v>
+      <c r="C18">
+        <f ca="1">+[1]Caja!$B$11/2</f>
+        <v>53</v>
       </c>
       <c r="D18" t="s">
         <v>14</v>
@@ -1148,9 +1207,9 @@
       <c r="A19" s="2">
         <v>44186</v>
       </c>
-      <c r="B19">
-        <f ca="1">+Caja!$B$11/2</f>
-        <v>50</v>
+      <c r="C19">
+        <f ca="1">+[1]Caja!$B$11/2</f>
+        <v>53</v>
       </c>
       <c r="D19" t="s">
         <v>14</v>
@@ -1163,9 +1222,9 @@
       <c r="A20" s="2">
         <v>44187</v>
       </c>
-      <c r="B20">
-        <f ca="1">+Caja!$B$12/2</f>
-        <v>56.5</v>
+      <c r="C20">
+        <f ca="1">+[1]Caja!$B$12/2</f>
+        <v>57.5</v>
       </c>
       <c r="D20" t="s">
         <v>14</v>
@@ -1178,9 +1237,9 @@
       <c r="A21" s="2">
         <v>44188</v>
       </c>
-      <c r="B21">
-        <f ca="1">+Caja!$B$12/2</f>
-        <v>56.5</v>
+      <c r="C21">
+        <f ca="1">+[1]Caja!$B$12/2</f>
+        <v>57.5</v>
       </c>
       <c r="D21" t="s">
         <v>14</v>
@@ -1193,9 +1252,9 @@
       <c r="A22" s="2">
         <v>44189</v>
       </c>
-      <c r="B22">
-        <f ca="1">+Caja!B13-37</f>
-        <v>70</v>
+      <c r="C22">
+        <f ca="1">+[1]Caja!B13-37</f>
+        <v>72</v>
       </c>
       <c r="D22" t="s">
         <v>16</v>
@@ -1208,7 +1267,7 @@
       <c r="A23" s="2">
         <v>44190</v>
       </c>
-      <c r="B23">
+      <c r="C23">
         <v>37</v>
       </c>
       <c r="D23" t="s">
@@ -1222,9 +1281,9 @@
       <c r="A24" s="2">
         <v>44191</v>
       </c>
-      <c r="B24">
-        <f ca="1">+Caja!B14-56</f>
-        <v>35</v>
+      <c r="C24">
+        <f ca="1">+[1]Caja!B14-56</f>
+        <v>58</v>
       </c>
       <c r="D24" t="s">
         <v>17</v>
@@ -1237,7 +1296,7 @@
       <c r="A25" s="2">
         <v>44192</v>
       </c>
-      <c r="B25">
+      <c r="C25">
         <v>56</v>
       </c>
       <c r="D25" t="s">
@@ -1251,7 +1310,7 @@
       <c r="A26" s="2">
         <v>44193</v>
       </c>
-      <c r="C26">
+      <c r="B26">
         <v>7.5</v>
       </c>
       <c r="D26" t="s">
@@ -1265,7 +1324,7 @@
       <c r="A27" s="2">
         <v>44194</v>
       </c>
-      <c r="B27">
+      <c r="C27">
         <v>320</v>
       </c>
       <c r="D27" t="s">
@@ -1279,7 +1338,7 @@
       <c r="A28" s="2">
         <v>44195</v>
       </c>
-      <c r="B28">
+      <c r="C28">
         <v>470</v>
       </c>
       <c r="D28" t="s">
@@ -1293,7 +1352,7 @@
       <c r="A29" s="2">
         <v>44196</v>
       </c>
-      <c r="B29">
+      <c r="C29">
         <v>75</v>
       </c>
       <c r="D29" t="s">
@@ -1307,7 +1366,7 @@
       <c r="A30" s="2">
         <v>44184</v>
       </c>
-      <c r="B30">
+      <c r="C30">
         <v>39</v>
       </c>
       <c r="D30" t="s">
@@ -1321,7 +1380,7 @@
       <c r="A31" s="2">
         <v>44185</v>
       </c>
-      <c r="B31">
+      <c r="C31">
         <v>1500</v>
       </c>
       <c r="D31" t="s">
@@ -1335,7 +1394,7 @@
       <c r="A32" s="2">
         <v>44186</v>
       </c>
-      <c r="B32">
+      <c r="C32">
         <v>1500</v>
       </c>
       <c r="D32" t="s">
@@ -1349,7 +1408,7 @@
       <c r="A33" s="2">
         <v>44187</v>
       </c>
-      <c r="B33">
+      <c r="C33">
         <v>1500</v>
       </c>
       <c r="D33" t="s">
@@ -1363,7 +1422,7 @@
       <c r="A34" s="2">
         <v>44188</v>
       </c>
-      <c r="B34">
+      <c r="C34">
         <v>1500</v>
       </c>
       <c r="D34" t="s">
@@ -1377,7 +1436,7 @@
       <c r="A35" s="2">
         <v>44189</v>
       </c>
-      <c r="B35">
+      <c r="C35">
         <v>1500</v>
       </c>
       <c r="D35" t="s">
@@ -1391,7 +1450,7 @@
       <c r="A36" s="2">
         <v>44190</v>
       </c>
-      <c r="B36">
+      <c r="C36">
         <v>1500</v>
       </c>
       <c r="D36" t="s">
@@ -1405,7 +1464,7 @@
       <c r="A37" s="2">
         <v>44191</v>
       </c>
-      <c r="B37">
+      <c r="C37">
         <v>1500</v>
       </c>
       <c r="D37" t="s">
@@ -1419,7 +1478,7 @@
       <c r="A38" s="2">
         <v>44192</v>
       </c>
-      <c r="B38">
+      <c r="C38">
         <v>1500</v>
       </c>
       <c r="D38" t="s">
@@ -1433,7 +1492,7 @@
       <c r="A39" s="2">
         <v>44193</v>
       </c>
-      <c r="B39">
+      <c r="C39">
         <v>127.99</v>
       </c>
       <c r="D39" t="s">
@@ -1447,7 +1506,7 @@
       <c r="A40" s="2">
         <v>44194</v>
       </c>
-      <c r="B40">
+      <c r="C40">
         <v>83</v>
       </c>
       <c r="D40" t="s">
@@ -1461,7 +1520,7 @@
       <c r="A41" s="2">
         <v>44195</v>
       </c>
-      <c r="C41">
+      <c r="B41">
         <v>6.35</v>
       </c>
       <c r="D41" t="s">
@@ -1475,7 +1534,7 @@
       <c r="A42" s="2">
         <v>44196</v>
       </c>
-      <c r="B42">
+      <c r="C42">
         <v>1.27</v>
       </c>
       <c r="D42" t="s">
@@ -1489,7 +1548,7 @@
       <c r="A43" s="2">
         <v>44196</v>
       </c>
-      <c r="B43">
+      <c r="C43">
         <v>12.5</v>
       </c>
       <c r="D43" t="s">
@@ -1503,7 +1562,7 @@
       <c r="A44" s="2">
         <v>44196</v>
       </c>
-      <c r="B44">
+      <c r="C44">
         <v>6.75</v>
       </c>
       <c r="D44" t="s">

</xml_diff>